<commit_message>
added the information about stride
</commit_message>
<xml_diff>
--- a/usenix_18.xlsx
+++ b/usenix_18.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29e1f5b82a02f9e3/Paper/usenix_18/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiaowan Dong\OneDrive\Paper\VEE_16\git-hub\sva_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="4C3259C6DFF952AB48E0EC6803DCB0802E782071" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{C6A3408E-DD6B-4824-92EC-D02FD50F8064}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="4C3259C6DFF952AB48E0EC6803DCB0802E782071" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{C90B0FE0-D5EF-41A8-B99A-6513DE1C7BB2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985" xr2:uid="{298021B8-ADE5-4423-814F-F76116AE5EDA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>LMBench</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>average (in microseconds)</t>
+  </si>
+  <si>
+    <t>stride = 64B</t>
   </si>
 </sst>
 </file>
@@ -2097,7 +2100,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2168,6 +2171,9 @@
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">

</xml_diff>